<commit_message>
Corrección en parseo de Renta Fija y Venta Simultanea.
Para la renta fija no hay que considerar los que dicen Retrov Nominal, y para la venta de simultaneas no se estaba haciendo el cálculo para determinar el valor de la cantidad.
</commit_message>
<xml_diff>
--- a/Nevasa/InformeCompleto/20240829/20240829_informe_completo_results.xlsx
+++ b/Nevasa/InformeCompleto/20240829/20240829_informe_completo_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1022,30 +1022,30 @@
         <v>45533</v>
       </c>
       <c r="D15" t="n">
-        <v>5.7071</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>865000000</v>
+        <v>12639064.464</v>
       </c>
       <c r="F15" t="n">
-        <v>907744334</v>
+        <v>12591214</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>BTP0600433</t>
+          <t>LTM</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>COMPRA</t>
+          <t>VENTA</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>RENTA FIJA</t>
+          <t>SIMULTANEA</t>
         </is>
       </c>
     </row>
@@ -1062,30 +1062,30 @@
         <v>45533</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>16406.72</v>
       </c>
       <c r="E16" t="n">
-        <v>12591214</v>
+        <v>8515</v>
       </c>
       <c r="F16" t="n">
-        <v>12591214</v>
+        <v>139703220</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>LTM</t>
+          <t>CFINHRFLA</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>VENTA</t>
+          <t>COMPRA</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>SIMULTANEA</t>
+          <t>RENTA VARIABLE</t>
         </is>
       </c>
     </row>
@@ -1105,10 +1105,10 @@
         <v>16406.72</v>
       </c>
       <c r="E17" t="n">
-        <v>8515</v>
+        <v>12673</v>
       </c>
       <c r="F17" t="n">
-        <v>139703220</v>
+        <v>207922363</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
@@ -1120,7 +1120,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>COMPRA</t>
+          <t>VENTA</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1142,25 +1142,25 @@
         <v>45533</v>
       </c>
       <c r="D18" t="n">
-        <v>16406.72</v>
+        <v>15850.56</v>
       </c>
       <c r="E18" t="n">
-        <v>12673</v>
+        <v>1199</v>
       </c>
       <c r="F18" t="n">
-        <v>207922363</v>
+        <v>19004821</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>CFINHRFLA</t>
+          <t>CFINHRFLB</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>VENTA</t>
+          <t>COMPRA</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1188,7 +1188,7 @@
         <v>1199</v>
       </c>
       <c r="F19" t="n">
-        <v>19004821</v>
+        <v>19004822</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
@@ -1200,50 +1200,10 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>COMPRA</t>
+          <t>VENTA</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
-        <is>
-          <t>RENTA VARIABLE</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>FONDO DE INVERSION NEVASA AHORRO</t>
-        </is>
-      </c>
-      <c r="B20" s="2" t="n">
-        <v>45533</v>
-      </c>
-      <c r="C20" s="2" t="n">
-        <v>45533</v>
-      </c>
-      <c r="D20" t="n">
-        <v>15850.56</v>
-      </c>
-      <c r="E20" t="n">
-        <v>1199</v>
-      </c>
-      <c r="F20" t="n">
-        <v>19004822</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0</v>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>CFINHRFLB</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>VENTA</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
         <is>
           <t>RENTA VARIABLE</t>
         </is>

</xml_diff>